<commit_message>
[master] finished php tutorial 5
</commit_message>
<xml_diff>
--- a/tutorials/tutorial_05/sample.xlsx
+++ b/tutorials/tutorial_05/sample.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
-  <si>
-    <t>HeinHtetSan</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>09-11111111</t>
   </si>
@@ -51,6 +48,39 @@
   </si>
   <si>
     <t>09-11111117</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Phone no</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>hla hla</t>
+  </si>
+  <si>
+    <t>ko ko</t>
+  </si>
+  <si>
+    <t>mg mg</t>
+  </si>
+  <si>
+    <t>nu nu</t>
+  </si>
+  <si>
+    <t>myo myo</t>
+  </si>
+  <si>
+    <t>soe soe</t>
+  </si>
+  <si>
+    <t>kyaw kyaw</t>
   </si>
 </sst>
 </file>
@@ -74,7 +104,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -82,12 +112,119 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -368,114 +505,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D3" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D4" s="6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="D6" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="D7" s="6">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7">
-        <v>25</v>
+      <c r="D8" s="9">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>